<commit_message>
adds fixed scraper data
</commit_message>
<xml_diff>
--- a/data/buyuksehir_belediyeleri.xlsx
+++ b/data/buyuksehir_belediyeleri.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ihp/Desktop/belediye/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ihp/Documents/Deve/Reddit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D991A544-85FE-A849-A507-E59E30AF9F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C871ED-CF11-2246-8533-73BAA7743A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17100" yWindow="6280" windowWidth="31220" windowHeight="24040" xr2:uid="{57379D8C-FED7-4946-B8CF-BC79304075E4}"/>
   </bookViews>
@@ -164,9 +164,6 @@
     <t>https://www.eskisehir.bel.tr</t>
   </si>
   <si>
-    <t>www.gaziantep.bel.tr</t>
-  </si>
-  <si>
     <t>https://hatay.bel.tr</t>
   </si>
   <si>
@@ -222,6 +219,9 @@
   </si>
   <si>
     <t>https://van.bel.tr</t>
+  </si>
+  <si>
+    <t>https://www.gaziantep.bel.tr/tr</t>
   </si>
 </sst>
 </file>
@@ -591,12 +591,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32E24E3-A682-D942-BD9E-AC2105A31847}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -700,7 +702,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -709,7 +711,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -718,7 +720,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -727,7 +729,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="2"/>
     </row>
@@ -736,7 +738,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -744,7 +746,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="2"/>
     </row>
@@ -753,7 +755,7 @@
         <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="2"/>
     </row>
@@ -762,7 +764,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="2"/>
     </row>
@@ -771,7 +773,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="2"/>
     </row>
@@ -780,7 +782,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -788,7 +790,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -796,7 +798,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -804,7 +806,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -812,7 +814,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="2"/>
     </row>
@@ -821,7 +823,7 @@
         <v>31</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="2"/>
     </row>
@@ -830,7 +832,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="2"/>
     </row>
@@ -839,7 +841,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C28" s="2"/>
     </row>
@@ -848,7 +850,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -856,7 +858,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -864,7 +866,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>